<commit_message>
Add some runs results
</commit_message>
<xml_diff>
--- a/developing/Results Homework DL.xlsx
+++ b/developing/Results Homework DL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesco\Documents\Scuola\Università\Materie Università\Anno 4\Deep Learning\Homework\Deep-Learning-Project\developing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634054C4-814C-4C49-BDA9-15B09C2BBEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6722713C-1A58-41E9-AEC4-D4060B03069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="12160" windowHeight="12693" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="142">
   <si>
     <t>No SMOTE, No Upsample</t>
   </si>
@@ -391,6 +391,66 @@
   </si>
   <si>
     <t>0.501646</t>
+  </si>
+  <si>
+    <t>0.976746</t>
+  </si>
+  <si>
+    <t>0.962360</t>
+  </si>
+  <si>
+    <t>0.968518</t>
+  </si>
+  <si>
+    <t>0.511215</t>
+  </si>
+  <si>
+    <t>0.968565</t>
+  </si>
+  <si>
+    <t>0.968057</t>
+  </si>
+  <si>
+    <t>0.968310</t>
+  </si>
+  <si>
+    <t>0.607393</t>
+  </si>
+  <si>
+    <t>0.487171</t>
+  </si>
+  <si>
+    <t>0.610248</t>
+  </si>
+  <si>
+    <t>0.959487</t>
+  </si>
+  <si>
+    <t>0.740531</t>
+  </si>
+  <si>
+    <t>0.510519</t>
+  </si>
+  <si>
+    <t>0.860438</t>
+  </si>
+  <si>
+    <t>0.958330</t>
+  </si>
+  <si>
+    <t>0.906091</t>
+  </si>
+  <si>
+    <t>0.473023</t>
+  </si>
+  <si>
+    <t>0.909976</t>
+  </si>
+  <si>
+    <t>0.933689</t>
+  </si>
+  <si>
+    <t>0.527398</t>
   </si>
 </sst>
 </file>
@@ -733,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -744,27 +804,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,7 +832,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1074,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1092,40 +1151,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="14" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="14" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="14" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="16"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="22"/>
     </row>
     <row r="2" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1188,10 +1247,10 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6"/>
@@ -1214,11 +1273,21 @@
       <c r="L3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="8"/>
+      <c r="M3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="R3" s="6" t="s">
         <v>61</v>
       </c>
@@ -1236,10 +1305,10 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9"/>
@@ -1262,11 +1331,21 @@
       <c r="L4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="2"/>
+      <c r="M4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="R4" s="9" t="s">
         <v>57</v>
       </c>
@@ -1284,10 +1363,10 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="9"/>
@@ -1310,11 +1389,21 @@
       <c r="L5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="2"/>
+      <c r="M5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="R5" s="9" t="s">
         <v>32</v>
       </c>
@@ -1332,8 +1421,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A6" s="25"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="9"/>
@@ -1356,11 +1445,21 @@
       <c r="L6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="2"/>
+      <c r="M6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="R6" s="9" t="s">
         <v>52</v>
       </c>
@@ -1378,8 +1477,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A7" s="25"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="9"/>
@@ -1402,11 +1501,21 @@
       <c r="L7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="2"/>
+      <c r="M7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="R7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1424,8 +1533,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="26"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
@@ -1448,11 +1557,21 @@
       <c r="L8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="4"/>
+      <c r="M8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="R8" s="5" t="s">
         <v>44</v>
       </c>
@@ -1471,40 +1590,40 @@
     </row>
     <row r="11" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="12" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="14" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="14" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="14" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="14" t="s">
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="16"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="22"/>
     </row>
     <row r="13" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1567,10 +1686,10 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="6"/>
@@ -1625,10 +1744,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="9"/>
@@ -1683,10 +1802,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="9"/>
@@ -1741,8 +1860,8 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A17" s="25"/>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="18"/>
+      <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="9"/>
@@ -1797,8 +1916,8 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="A18" s="25"/>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="9"/>
@@ -1853,8 +1972,8 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="26"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="5"/>
@@ -1909,10 +2028,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="M23" s="17"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="D27" s="27"/>
+      <c r="M23" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>